<commit_message>
Updating previous study intercomparisons sheet
</commit_message>
<xml_diff>
--- a/Planning_Methods/PreviousStudy_Intercomparison.xlsx
+++ b/Planning_Methods/PreviousStudy_Intercomparison.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.salkgundersen\Documents\GitHub_Repos\UtahLake_CNPMassBalance\Planning&amp;Methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.salkgundersen\Documents\GitHub_Repos\UtahLake_CNPMassBalance\Planning_Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810A2B97-D991-470C-B8AE-981567DBD893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1762E236-1093-49EA-9EFA-87261CF54448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="2010" windowWidth="23250" windowHeight="12570" xr2:uid="{1E3BBE6F-4AB7-4812-9983-36F4C365C34D}"/>
+    <workbookView xWindow="30960" yWindow="990" windowWidth="23250" windowHeight="14130" xr2:uid="{1E3BBE6F-4AB7-4812-9983-36F4C365C34D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Methods" sheetId="1" r:id="rId1"/>
+    <sheet name="Percentages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>PSOMAS and SWCA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="62">
   <si>
     <t>Merritt and Miller</t>
   </si>
@@ -50,15 +48,197 @@
     <t>Level of Uncertainty</t>
   </si>
   <si>
-    <t>Brett</t>
+    <t>Gaged stream inflows</t>
+  </si>
+  <si>
+    <t>USGS gages</t>
+  </si>
+  <si>
+    <t>Ungaged stream inflows</t>
+  </si>
+  <si>
+    <t>LKSIM</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>Evaporation</t>
+  </si>
+  <si>
+    <t>Groundwater</t>
+  </si>
+  <si>
+    <t>Spring inflow</t>
+  </si>
+  <si>
+    <t>Groundwater inflow</t>
+  </si>
+  <si>
+    <t>Surface drain inflow</t>
+  </si>
+  <si>
+    <t>Jordan River Outflow</t>
+  </si>
+  <si>
+    <t>WWTP inflow</t>
+  </si>
+  <si>
+    <t>POTW records</t>
+  </si>
+  <si>
+    <t>LKSIM via precipitation and correlation with gaged sites</t>
+  </si>
+  <si>
+    <t>Weather stations, interpolated via Theissen Polygon method</t>
+  </si>
+  <si>
+    <t>LKSIM by salt balance and salinity properties of thermal springs</t>
+  </si>
+  <si>
+    <t>LKSIM based on water balance</t>
+  </si>
+  <si>
+    <t>Groundwater outflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USGS gage </t>
+  </si>
+  <si>
+    <t>Morton model based on air temperature, humidity, and solar radiation</t>
+  </si>
+  <si>
+    <t>PSOMAS and SWCA methods</t>
+  </si>
+  <si>
+    <t>Percentage type</t>
+  </si>
+  <si>
+    <t>Stream inflow</t>
+  </si>
+  <si>
+    <t>Inflow</t>
+  </si>
+  <si>
+    <t>Groundwater and springs</t>
+  </si>
+  <si>
+    <t>Surface drains and overland flow</t>
+  </si>
+  <si>
+    <t>Jordan River outflow</t>
+  </si>
+  <si>
+    <t>Outflow</t>
+  </si>
+  <si>
+    <t>Concentration from STORET. If a month was not available, average of previous and next month taken. Assume unknown addition or removal is negligible.</t>
+  </si>
+  <si>
+    <t>Stream TP concentration (measured)</t>
+  </si>
+  <si>
+    <t>Stream TP concentration (unmeasured)</t>
+  </si>
+  <si>
+    <t>Flows grouped with similar watersheds, assigned TP concentration based on grab data/similar systems/literature/best professional judgement</t>
+  </si>
+  <si>
+    <t>Surface drain TP concentration</t>
+  </si>
+  <si>
+    <t>0.15 mg/L</t>
+  </si>
+  <si>
+    <t>Overland flow TP concentration</t>
+  </si>
+  <si>
+    <t>0.10 mg/L</t>
+  </si>
+  <si>
+    <t>Groundwater TP concentration</t>
+  </si>
+  <si>
+    <t>0.02 mg/L</t>
+  </si>
+  <si>
+    <t>WWTP TP concentration</t>
+  </si>
+  <si>
+    <t>WWTP discharge</t>
+  </si>
+  <si>
+    <t>Other inflows</t>
+  </si>
+  <si>
+    <t>TP load out</t>
+  </si>
+  <si>
+    <t>TP load in</t>
+  </si>
+  <si>
+    <t>Other outflows</t>
+  </si>
+  <si>
+    <t>Percentage (PSOMAS and SWCA 2007)</t>
+  </si>
+  <si>
+    <t>Percentage (Merritt and Miller 2016)</t>
+  </si>
+  <si>
+    <t>Stream inflow (including WWTP)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>DN load in</t>
+  </si>
+  <si>
+    <t>DP load in</t>
+  </si>
+  <si>
+    <t>Utah DWQ</t>
+  </si>
+  <si>
+    <t>LKSIM, direct measurements at major tribs</t>
+  </si>
+  <si>
+    <t>Jordan River/Utah Lake commissioner'</t>
+  </si>
+  <si>
+    <t>LKSIM via overall or seasonal means from larger tributaries estimated by eye by Dr. Merritt</t>
+  </si>
+  <si>
+    <t>DMR records</t>
+  </si>
+  <si>
+    <t>Water Quality Portal</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Drainage area ratio method, pair similar characteristics together</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,8 +266,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,39 +590,625 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1CF8655-910D-4AE3-8BAE-A6F4AC6FAF0D}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="5" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F74FDA8-6A50-4088-872A-34835E38B3C7}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="4" width="16.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>51</v>
+      </c>
+      <c r="D2" s="4">
+        <f>495092/646171*100</f>
+        <v>76.619346891148012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4">
+        <f>(43171+14744)/646171*100</f>
+        <v>8.9627977733448265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4">
+        <f>93164/646171*100</f>
+        <v>14.417855335507165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <f>336045/668853*100</f>
+        <v>50.241981421926795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <f>332808/668853*100</f>
+        <v>49.758018578073212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>76.5</v>
+      </c>
+      <c r="D9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>20.7</v>
+      </c>
+      <c r="D10">
+        <f>7+7.6+1.6+1.6</f>
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>2.8</v>
+      </c>
+      <c r="D11">
+        <f>0.5+0.4</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <f>14.5+17.5+5.5+2.3</f>
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <f>2.4+0.1</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <f>4.2+6.2+1.3+1.5</f>
+        <v>13.200000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21">
+        <f>0.4+0.3</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>